<commit_message>
Update conversatii.xlsx with new data
</commit_message>
<xml_diff>
--- a/conversatii.xlsx
+++ b/conversatii.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stas Tarnavskiy\OneDrive\Рабочий стол\chatbot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stas Tarnavskiy\OneDrive\Рабочий стол\Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3553F363-B81F-4F82-8584-FB6A9D9E5779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC415BA-148E-4EFD-9C8E-1D144DEBD706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Bot: Bună! Cum te cheamă?</t>
   </si>
@@ -37,10 +37,10 @@
     <t>Bot: Ce îți place să faci?</t>
   </si>
   <si>
-    <t>Tu: dans</t>
-  </si>
-  <si>
-    <t>Bot: Salut Stas! Este minunat că un tânăr dansează!</t>
+    <t>Tu: dans812</t>
+  </si>
+  <si>
+    <t>Bot: Salutare, Stas! Este minunat că un tânăr dansează!</t>
   </si>
   <si>
     <t>Bot: Vrei să continui conversația? (da/nu)</t>
@@ -52,25 +52,13 @@
     <t>Tu: Alex</t>
   </si>
   <si>
-    <t>Tu: 35</t>
-  </si>
-  <si>
-    <t>Tu: sah</t>
-  </si>
-  <si>
-    <t>Bot: Hei Alex! Este minunat că un adult se ocupă cu sah!</t>
-  </si>
-  <si>
-    <t>Tu: Nicu</t>
-  </si>
-  <si>
-    <t>Tu: 13</t>
+    <t>Tu: 37</t>
   </si>
   <si>
     <t>Tu: fotbal</t>
   </si>
   <si>
-    <t>Bot: Salutare, Nicu! Este minunat că un copil joacă fotbal!</t>
+    <t>Bot: Bună Alex! Este minunat că un adult joacă fotbal!</t>
   </si>
   <si>
     <t>Tu: nu</t>
@@ -413,15 +401,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -511,52 +497,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>